<commit_message>
updated figures and tables
</commit_message>
<xml_diff>
--- a/i_test/test_D3_study_population/D3_source_population.xlsx
+++ b/i_test/test_D3_study_population/D3_source_population.xlsx
@@ -46,12 +46,6 @@
     <t>treated</t>
   </si>
   <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>P01</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>P03</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,10 +477,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -494,13 +494,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>-30000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -511,13 +511,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>-30000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>600</v>
@@ -528,13 +528,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>-30000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
@@ -545,13 +545,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>-30000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -578,6 +578,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dac44d48b4406d5c320fe911a853389">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="183e839aabd2ef2c305af4a754f6d8de" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -822,15 +831,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
   <ds:schemaRefs>
@@ -849,6 +849,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC727D-6270-488A-9B63-C6970CF6C0A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -865,12 +873,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>